<commit_message>
✨ MaxShifts & opmerkingen uit Excel toegevoegd
</commit_message>
<xml_diff>
--- a/excel-hulpbestanden/beschikbaarheid-7.xlsx
+++ b/excel-hulpbestanden/beschikbaarheid-7.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\van den Akker\planner\planner-app\excel-hulpbestanden\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{115E3DBF-BDD7-44AE-9D6F-4ACA05FF4E65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEF0ED17-54EA-4364-BC02-645620F839DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="1800" windowWidth="29040" windowHeight="16440" xr2:uid="{441931CC-1960-4929-88FC-9E923128FEA4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{441931CC-1960-4929-88FC-9E923128FEA4}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="728" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="777" uniqueCount="92">
   <si>
     <t>Naam</t>
   </si>
@@ -290,13 +290,28 @@
     <t>Claire van Warmerdam</t>
   </si>
   <si>
-    <t>wo/vr later, tm 11 juli beschikbaar</t>
-  </si>
-  <si>
     <t>van 3/7 t/m 20/8 ma t/m do shift 1, vr t/m zo shift 2</t>
   </si>
   <si>
     <t>t/m  15 aug geldt dit</t>
+  </si>
+  <si>
+    <t>na ZF niet meer op vrijdag en na 25-8 helemaal niet meer</t>
+  </si>
+  <si>
+    <t>Vanaf augustus niet meer indelen (operatie)</t>
+  </si>
+  <si>
+    <t>wo/vr later, tm 11 juli beschikbaar, daarna niet meer</t>
+  </si>
+  <si>
+    <t>Lene te Molder</t>
+  </si>
+  <si>
+    <t>Tessa van Haren</t>
+  </si>
+  <si>
+    <t>Tyra Vroomen</t>
   </si>
 </sst>
 </file>
@@ -757,10 +772,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9E942E7-99C6-4731-BEC2-AED1E14052AD}">
-  <dimension ref="A1:S44"/>
+  <dimension ref="A1:S47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1195,7 +1210,9 @@
       <c r="D8" s="6">
         <v>39164</v>
       </c>
-      <c r="E8" s="1"/>
+      <c r="E8" s="1" t="s">
+        <v>86</v>
+      </c>
       <c r="F8" s="5" t="s">
         <v>23</v>
       </c>
@@ -1220,8 +1237,8 @@
       <c r="M8" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="N8" s="5" t="s">
-        <v>23</v>
+      <c r="N8" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="O8" s="4" t="s">
         <v>24</v>
@@ -1658,7 +1675,7 @@
         <v>39379</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>23</v>
@@ -1835,7 +1852,7 @@
         <v>39049</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>4</v>
+        <v>87</v>
       </c>
       <c r="F19" s="4" t="s">
         <v>24</v>
@@ -1953,7 +1970,7 @@
         <v>38635</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F21" s="5" t="s">
         <v>23</v>
@@ -2173,7 +2190,7 @@
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>45</v>
+        <v>89</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>6</v>
@@ -2182,11 +2199,9 @@
         <v>2</v>
       </c>
       <c r="D25" s="6">
-        <v>39220</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>84</v>
-      </c>
+        <v>38610</v>
+      </c>
+      <c r="E25" s="1"/>
       <c r="F25" s="4" t="s">
         <v>24</v>
       </c>
@@ -2196,11 +2211,11 @@
       <c r="H25" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="I25" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="J25" s="5" t="s">
-        <v>23</v>
+      <c r="I25" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="J25" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="K25" s="4" t="s">
         <v>24</v>
@@ -2211,8 +2226,8 @@
       <c r="M25" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="N25" s="5" t="s">
-        <v>23</v>
+      <c r="N25" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="O25" s="5" t="s">
         <v>23</v>
@@ -2226,24 +2241,26 @@
       <c r="R25" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="S25" s="4" t="s">
-        <v>24</v>
+      <c r="S25" s="5" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C26" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D26" s="6">
-        <v>40481</v>
-      </c>
-      <c r="E26" s="1"/>
+        <v>39220</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>88</v>
+      </c>
       <c r="F26" s="4" t="s">
         <v>24</v>
       </c>
@@ -2280,8 +2297,8 @@
       <c r="Q26" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="R26" s="5" t="s">
-        <v>23</v>
+      <c r="R26" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="S26" s="4" t="s">
         <v>24</v>
@@ -2289,29 +2306,29 @@
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C27" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D27" s="6">
-        <v>39402</v>
+        <v>40481</v>
       </c>
       <c r="E27" s="1"/>
       <c r="F27" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="G27" s="5" t="s">
-        <v>23</v>
+      <c r="G27" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="H27" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="I27" s="5" t="s">
-        <v>23</v>
+      <c r="I27" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="J27" s="4" t="s">
         <v>24</v>
@@ -2331,44 +2348,44 @@
       <c r="O27" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="P27" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q27" s="5" t="s">
-        <v>23</v>
+      <c r="P27" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q27" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="R27" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="S27" s="5" t="s">
-        <v>23</v>
+      <c r="S27" s="4" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C28" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D28" s="6">
-        <v>40452</v>
+        <v>39402</v>
       </c>
       <c r="E28" s="1"/>
       <c r="F28" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="G28" s="4" t="s">
-        <v>24</v>
+      <c r="G28" s="5" t="s">
+        <v>23</v>
       </c>
       <c r="H28" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="I28" s="4" t="s">
-        <v>24</v>
+      <c r="I28" s="5" t="s">
+        <v>23</v>
       </c>
       <c r="J28" s="4" t="s">
         <v>24</v>
@@ -2388,31 +2405,31 @@
       <c r="O28" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="P28" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q28" s="4" t="s">
-        <v>24</v>
+      <c r="P28" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q28" s="5" t="s">
+        <v>23</v>
       </c>
       <c r="R28" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="S28" s="4" t="s">
-        <v>24</v>
+      <c r="S28" s="5" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>47</v>
+        <v>81</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C29" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D29" s="6">
-        <v>39276</v>
+        <v>40452</v>
       </c>
       <c r="E29" s="1"/>
       <c r="F29" s="4" t="s">
@@ -2421,8 +2438,8 @@
       <c r="G29" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="H29" s="5" t="s">
-        <v>23</v>
+      <c r="H29" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="I29" s="4" t="s">
         <v>24</v>
@@ -2433,8 +2450,8 @@
       <c r="K29" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="L29" s="5" t="s">
-        <v>23</v>
+      <c r="L29" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="M29" s="4" t="s">
         <v>24</v>
@@ -2451,8 +2468,8 @@
       <c r="Q29" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="R29" s="4" t="s">
-        <v>24</v>
+      <c r="R29" s="5" t="s">
+        <v>23</v>
       </c>
       <c r="S29" s="4" t="s">
         <v>24</v>
@@ -2460,22 +2477,20 @@
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C30" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D30" s="6">
-        <v>38353</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F30" s="5" t="s">
-        <v>23</v>
+        <v>39276</v>
+      </c>
+      <c r="E30" s="1"/>
+      <c r="F30" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="G30" s="4" t="s">
         <v>24</v>
@@ -2483,11 +2498,11 @@
       <c r="H30" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I30" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="J30" s="5" t="s">
-        <v>23</v>
+      <c r="I30" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="J30" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="K30" s="4" t="s">
         <v>24</v>
@@ -2495,74 +2510,76 @@
       <c r="L30" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="M30" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="N30" s="5" t="s">
-        <v>23</v>
+      <c r="M30" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="N30" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="O30" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="P30" s="5" t="s">
-        <v>23</v>
+      <c r="P30" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="Q30" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="R30" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="S30" s="5" t="s">
-        <v>23</v>
+      <c r="R30" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="S30" s="4" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C31" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D31" s="6">
-        <v>40451</v>
-      </c>
-      <c r="E31" s="1"/>
-      <c r="F31" s="4" t="s">
-        <v>24</v>
+        <v>38353</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>23</v>
       </c>
       <c r="G31" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="H31" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="I31" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="J31" s="4" t="s">
-        <v>24</v>
+      <c r="H31" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I31" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="J31" s="5" t="s">
+        <v>23</v>
       </c>
       <c r="K31" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="L31" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="M31" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="N31" s="4" t="s">
-        <v>24</v>
+      <c r="L31" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="M31" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="N31" s="5" t="s">
+        <v>23</v>
       </c>
       <c r="O31" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="P31" s="4" t="s">
-        <v>24</v>
+      <c r="P31" s="5" t="s">
+        <v>23</v>
       </c>
       <c r="Q31" s="4" t="s">
         <v>24</v>
@@ -2570,29 +2587,29 @@
       <c r="R31" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="S31" s="4" t="s">
-        <v>24</v>
+      <c r="S31" s="5" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C32" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D32" s="6">
-        <v>38538</v>
+        <v>40451</v>
       </c>
       <c r="E32" s="1"/>
-      <c r="F32" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="G32" s="5" t="s">
-        <v>23</v>
+      <c r="F32" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="H32" s="4" t="s">
         <v>24</v>
@@ -2600,32 +2617,32 @@
       <c r="I32" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="J32" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="K32" s="5" t="s">
-        <v>23</v>
+      <c r="J32" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="K32" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="L32" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="M32" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="N32" s="5" t="s">
-        <v>23</v>
+      <c r="M32" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="N32" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="O32" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="P32" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q32" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="R32" s="4" t="s">
-        <v>24</v>
+      <c r="P32" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q32" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="R32" s="5" t="s">
+        <v>23</v>
       </c>
       <c r="S32" s="4" t="s">
         <v>24</v>
@@ -2633,23 +2650,23 @@
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C33" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D33" s="6">
-        <v>40114</v>
+        <v>38538</v>
       </c>
       <c r="E33" s="1"/>
-      <c r="F33" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G33" s="4" t="s">
-        <v>24</v>
+      <c r="F33" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>23</v>
       </c>
       <c r="H33" s="4" t="s">
         <v>24</v>
@@ -2657,32 +2674,32 @@
       <c r="I33" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="J33" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="K33" s="4" t="s">
-        <v>24</v>
+      <c r="J33" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="K33" s="5" t="s">
+        <v>23</v>
       </c>
       <c r="L33" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="M33" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="N33" s="4" t="s">
-        <v>24</v>
+      <c r="M33" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="N33" s="5" t="s">
+        <v>23</v>
       </c>
       <c r="O33" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="P33" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q33" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="R33" s="5" t="s">
-        <v>23</v>
+      <c r="P33" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q33" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="R33" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="S33" s="4" t="s">
         <v>24</v>
@@ -2690,25 +2707,23 @@
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C34" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D34" s="6">
-        <v>39674</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>77</v>
-      </c>
+        <v>40114</v>
+      </c>
+      <c r="E34" s="1"/>
       <c r="F34" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="G34" s="5" t="s">
-        <v>23</v>
+      <c r="G34" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="H34" s="4" t="s">
         <v>24</v>
@@ -2719,8 +2734,8 @@
       <c r="J34" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="K34" s="5" t="s">
-        <v>23</v>
+      <c r="K34" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="L34" s="4" t="s">
         <v>24</v>
@@ -2734,22 +2749,22 @@
       <c r="O34" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="P34" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q34" s="5" t="s">
-        <v>23</v>
+      <c r="P34" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q34" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="R34" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="S34" s="5" t="s">
-        <v>23</v>
+      <c r="S34" s="4" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>82</v>
+        <v>50</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>6</v>
@@ -2758,14 +2773,16 @@
         <v>2</v>
       </c>
       <c r="D35" s="6">
-        <v>39636</v>
-      </c>
-      <c r="E35" s="1"/>
+        <v>39674</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>77</v>
+      </c>
       <c r="F35" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="G35" s="4" t="s">
-        <v>24</v>
+      <c r="G35" s="5" t="s">
+        <v>23</v>
       </c>
       <c r="H35" s="4" t="s">
         <v>24</v>
@@ -2776,14 +2793,14 @@
       <c r="J35" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="K35" s="4" t="s">
-        <v>24</v>
+      <c r="K35" s="5" t="s">
+        <v>23</v>
       </c>
       <c r="L35" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="M35" s="5" t="s">
-        <v>23</v>
+      <c r="M35" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="N35" s="4" t="s">
         <v>24</v>
@@ -2797,50 +2814,50 @@
       <c r="Q35" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="R35" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="S35" s="4" t="s">
-        <v>24</v>
+      <c r="R35" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="S35" s="5" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C36" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D36" s="6">
-        <v>39762</v>
+        <v>39636</v>
       </c>
       <c r="E36" s="1"/>
-      <c r="F36" s="5" t="s">
-        <v>23</v>
+      <c r="F36" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="G36" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="H36" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="I36" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="J36" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="K36" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="L36" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="M36" s="4" t="s">
-        <v>24</v>
+      <c r="H36" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I36" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="J36" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="K36" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="L36" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="M36" s="5" t="s">
+        <v>23</v>
       </c>
       <c r="N36" s="4" t="s">
         <v>24</v>
@@ -2848,31 +2865,31 @@
       <c r="O36" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="P36" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q36" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="R36" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="S36" s="5" t="s">
-        <v>23</v>
+      <c r="P36" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q36" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="R36" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="S36" s="4" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>51</v>
+        <v>80</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C37" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D37" s="6">
-        <v>38392</v>
+        <v>39762</v>
       </c>
       <c r="E37" s="1"/>
       <c r="F37" s="5" t="s">
@@ -2881,20 +2898,20 @@
       <c r="G37" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="H37" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="I37" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="J37" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="K37" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="L37" s="4" t="s">
-        <v>24</v>
+      <c r="H37" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I37" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="J37" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="K37" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="L37" s="5" t="s">
+        <v>23</v>
       </c>
       <c r="M37" s="4" t="s">
         <v>24</v>
@@ -2911,8 +2928,8 @@
       <c r="Q37" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="R37" s="4" t="s">
-        <v>24</v>
+      <c r="R37" s="5" t="s">
+        <v>23</v>
       </c>
       <c r="S37" s="5" t="s">
         <v>23</v>
@@ -2920,22 +2937,20 @@
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C38" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D38" s="6">
-        <v>38547</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F38" s="4" t="s">
-        <v>24</v>
+        <v>38392</v>
+      </c>
+      <c r="E38" s="1"/>
+      <c r="F38" s="5" t="s">
+        <v>23</v>
       </c>
       <c r="G38" s="4" t="s">
         <v>24</v>
@@ -2964,8 +2979,8 @@
       <c r="O38" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="P38" s="5" t="s">
-        <v>23</v>
+      <c r="P38" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="Q38" s="4" t="s">
         <v>24</v>
@@ -2973,50 +2988,52 @@
       <c r="R38" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="S38" s="4" t="s">
-        <v>24</v>
+      <c r="S38" s="5" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C39" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D39" s="6">
-        <v>37817</v>
-      </c>
-      <c r="E39" s="1"/>
-      <c r="F39" s="5" t="s">
-        <v>23</v>
+        <v>38547</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="G39" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="H39" s="5" t="s">
-        <v>23</v>
+      <c r="H39" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="I39" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="J39" s="5" t="s">
-        <v>23</v>
+      <c r="J39" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="K39" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="L39" s="5" t="s">
-        <v>23</v>
+      <c r="L39" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="M39" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="N39" s="5" t="s">
-        <v>23</v>
+      <c r="N39" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="O39" s="4" t="s">
         <v>24</v>
@@ -3027,8 +3044,8 @@
       <c r="Q39" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="R39" s="5" t="s">
-        <v>23</v>
+      <c r="R39" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="S39" s="4" t="s">
         <v>24</v>
@@ -3036,7 +3053,7 @@
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>6</v>
@@ -3045,28 +3062,26 @@
         <v>4</v>
       </c>
       <c r="D40" s="6">
-        <v>38183</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F40" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G40" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H40" s="4" t="s">
-        <v>24</v>
+        <v>37817</v>
+      </c>
+      <c r="E40" s="1"/>
+      <c r="F40" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G40" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H40" s="5" t="s">
+        <v>23</v>
       </c>
       <c r="I40" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="J40" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="K40" s="5" t="s">
-        <v>23</v>
+      <c r="J40" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="K40" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="L40" s="5" t="s">
         <v>23</v>
@@ -3086,8 +3101,8 @@
       <c r="Q40" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="R40" s="4" t="s">
-        <v>24</v>
+      <c r="R40" s="5" t="s">
+        <v>23</v>
       </c>
       <c r="S40" s="4" t="s">
         <v>24</v>
@@ -3095,32 +3110,34 @@
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>78</v>
+        <v>54</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C41" s="3">
+        <v>4</v>
+      </c>
+      <c r="D41" s="6">
+        <v>38183</v>
+      </c>
+      <c r="E41" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D41" s="6">
-        <v>38317</v>
-      </c>
-      <c r="E41" s="1"/>
-      <c r="F41" s="5" t="s">
-        <v>23</v>
+      <c r="F41" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="G41" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="H41" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="I41" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="J41" s="5" t="s">
-        <v>23</v>
+      <c r="H41" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I41" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="J41" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="K41" s="5" t="s">
         <v>23</v>
@@ -3128,59 +3145,59 @@
       <c r="L41" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="M41" s="5" t="s">
-        <v>23</v>
+      <c r="M41" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="N41" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="O41" s="5" t="s">
-        <v>23</v>
+      <c r="O41" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="P41" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="Q41" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="R41" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="S41" s="5" t="s">
-        <v>23</v>
+      <c r="Q41" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="R41" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="S41" s="4" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C42" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D42" s="6">
-        <v>37364</v>
+        <v>38317</v>
       </c>
       <c r="E42" s="1"/>
-      <c r="F42" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G42" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="H42" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="I42" s="4" t="s">
-        <v>24</v>
+      <c r="F42" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G42" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H42" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I42" s="5" t="s">
+        <v>23</v>
       </c>
       <c r="J42" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="K42" s="4" t="s">
-        <v>24</v>
+      <c r="K42" s="5" t="s">
+        <v>23</v>
       </c>
       <c r="L42" s="5" t="s">
         <v>23</v>
@@ -3191,25 +3208,25 @@
       <c r="N42" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="O42" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="P42" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q42" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="R42" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="S42" s="4" t="s">
-        <v>24</v>
+      <c r="O42" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="P42" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q42" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="R42" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="S42" s="5" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>63</v>
+        <v>90</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>6</v>
@@ -3218,37 +3235,35 @@
         <v>2</v>
       </c>
       <c r="D43" s="6">
-        <v>38911</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>64</v>
-      </c>
+        <v>37448</v>
+      </c>
+      <c r="E43" s="1"/>
       <c r="F43" s="5" t="s">
         <v>23</v>
       </c>
       <c r="G43" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="H43" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="I43" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="J43" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="K43" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="L43" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="M43" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="N43" s="5" t="s">
-        <v>23</v>
+      <c r="H43" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I43" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="J43" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="K43" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="L43" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="M43" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="N43" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="O43" s="4" t="s">
         <v>24</v>
@@ -3259,75 +3274,248 @@
       <c r="Q43" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="R43" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="S43" s="5" t="s">
-        <v>23</v>
+      <c r="R43" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="S43" s="4" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C44" s="3">
+        <v>2</v>
+      </c>
+      <c r="D44" s="6">
+        <v>37364</v>
+      </c>
+      <c r="E44" s="1"/>
+      <c r="F44" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G44" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H44" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I44" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="J44" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="K44" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="L44" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="M44" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="N44" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="O44" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P44" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q44" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="R44" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="S44" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C45" s="3">
+        <v>4</v>
+      </c>
+      <c r="D45" s="6">
+        <v>38485</v>
+      </c>
+      <c r="E45" s="1"/>
+      <c r="F45" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G45" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H45" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I45" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="J45" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="K45" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="L45" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="M45" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="N45" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O45" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="P45" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q45" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="R45" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="S45" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C46" s="3">
+        <v>2</v>
+      </c>
+      <c r="D46" s="6">
+        <v>38911</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F46" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G46" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H46" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I46" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="J46" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="K46" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="L46" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="M46" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="N46" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="O46" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P46" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q46" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="R46" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="S46" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B44" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C44" s="3">
+      <c r="B47" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C47" s="3">
         <v>1</v>
       </c>
-      <c r="D44" s="6">
+      <c r="D47" s="6">
         <v>38268</v>
       </c>
-      <c r="E44" s="1" t="s">
+      <c r="E47" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="F44" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G44" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H44" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="I44" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="J44" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="K44" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="L44" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="M44" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="N44" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="O44" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="P44" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q44" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="R44" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="S44" s="4" t="s">
+      <c r="F47" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G47" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H47" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I47" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="J47" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="K47" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="L47" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="M47" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="N47" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O47" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P47" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q47" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="R47" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="S47" s="4" t="s">
         <v>24</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A12:S44">
-    <sortCondition ref="A12:A44"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A12:S47">
+    <sortCondition ref="A12:A47"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>